<commit_message>
created feature: was created file in the project to create the geometric conformity chart
</commit_message>
<xml_diff>
--- a/dados/peca_1/analise.xlsx
+++ b/dados/peca_1/analise.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L121"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -595,7 +595,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -647,7 +647,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -699,7 +699,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -763,7 +763,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -867,7 +867,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -919,7 +919,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -946,10 +946,10 @@
         <v>-588.9299999999999</v>
       </c>
       <c r="H10" t="n">
-        <v>-589.1799999999999</v>
+        <v>-589.28</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.25</v>
+        <v>-0.35</v>
       </c>
       <c r="J10" t="n">
         <v>0.5</v>
@@ -959,7 +959,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -998,10 +998,10 @@
         <v>-435.87</v>
       </c>
       <c r="H11" t="n">
-        <v>-435.89</v>
+        <v>-435.88</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="J11" t="n">
         <v>0.5</v>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1050,10 +1050,10 @@
         <v>-39.78</v>
       </c>
       <c r="H12" t="n">
-        <v>-40.1</v>
+        <v>-40.07</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.31</v>
+        <v>-0.28</v>
       </c>
       <c r="J12" t="n">
         <v>0.5</v>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21:11:32</t>
+          <t>22:10:58</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1102,10 +1102,10 @@
         <v>6.5</v>
       </c>
       <c r="H13" t="n">
-        <v>6.73</v>
+        <v>6.74</v>
       </c>
       <c r="I13" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="J13" t="n">
         <v>0.08</v>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>C2605.TXT</t>
+          <t>C2608.TXT</t>
         </is>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1570,10 +1570,10 @@
         <v>-588.9299999999999</v>
       </c>
       <c r="H22" t="n">
-        <v>-589.21</v>
+        <v>-589.16</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.28</v>
+        <v>-0.23</v>
       </c>
       <c r="J22" t="n">
         <v>0.5</v>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1622,10 +1622,10 @@
         <v>-435.87</v>
       </c>
       <c r="H23" t="n">
-        <v>-435.88</v>
+        <v>-435.91</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="J23" t="n">
         <v>0.5</v>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1674,10 +1674,10 @@
         <v>-39.78</v>
       </c>
       <c r="H24" t="n">
-        <v>-40.09</v>
+        <v>-40.11</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.31</v>
+        <v>-0.33</v>
       </c>
       <c r="J24" t="n">
         <v>0.5</v>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>21:51:12</t>
+          <t>22:17:40</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1726,10 +1726,10 @@
         <v>6.5</v>
       </c>
       <c r="H25" t="n">
-        <v>6.73</v>
+        <v>6.74</v>
       </c>
       <c r="I25" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="J25" t="n">
         <v>0.08</v>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>C2606.TXT</t>
+          <t>C2609.TXT</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2207,7 +2207,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2246,10 +2246,10 @@
         <v>-435.87</v>
       </c>
       <c r="H35" t="n">
-        <v>-435.86</v>
+        <v>-435.89</v>
       </c>
       <c r="I35" t="n">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="J35" t="n">
         <v>0.5</v>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -2271,7 +2271,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2298,10 +2298,10 @@
         <v>-39.78</v>
       </c>
       <c r="H36" t="n">
-        <v>-40.07</v>
+        <v>-40.1</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.29</v>
+        <v>-0.32</v>
       </c>
       <c r="J36" t="n">
         <v>0.5</v>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>22:00:41</t>
+          <t>22:25:35</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2350,10 +2350,10 @@
         <v>6.5</v>
       </c>
       <c r="H37" t="n">
-        <v>6.74</v>
+        <v>6.77</v>
       </c>
       <c r="I37" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="J37" t="n">
         <v>0.08</v>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>C2607.TXT</t>
+          <t>C2610.TXT</t>
         </is>
       </c>
     </row>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2415,7 +2415,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2519,7 +2519,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2818,10 +2818,10 @@
         <v>-588.9299999999999</v>
       </c>
       <c r="H46" t="n">
-        <v>-589.28</v>
+        <v>-588.91</v>
       </c>
       <c r="I46" t="n">
-        <v>-0.35</v>
+        <v>0.02</v>
       </c>
       <c r="J46" t="n">
         <v>0.5</v>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2873,7 +2873,7 @@
         <v>-435.88</v>
       </c>
       <c r="I47" t="n">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="J47" t="n">
         <v>0.5</v>
@@ -2883,7 +2883,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2922,10 +2922,10 @@
         <v>-39.78</v>
       </c>
       <c r="H48" t="n">
-        <v>-40.07</v>
+        <v>-40.05</v>
       </c>
       <c r="I48" t="n">
-        <v>-0.28</v>
+        <v>-0.27</v>
       </c>
       <c r="J48" t="n">
         <v>0.5</v>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>22:10:58</t>
+          <t>22:36:51</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2974,10 +2974,10 @@
         <v>6.5</v>
       </c>
       <c r="H49" t="n">
-        <v>6.74</v>
+        <v>6.73</v>
       </c>
       <c r="I49" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="J49" t="n">
         <v>0.08</v>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>C2608.TXT</t>
+          <t>C2611.TXT</t>
         </is>
       </c>
     </row>
@@ -2999,7 +2999,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3039,7 +3039,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3103,7 +3103,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3247,7 +3247,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3351,7 +3351,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3363,7 +3363,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3403,7 +3403,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3442,10 +3442,10 @@
         <v>-588.9299999999999</v>
       </c>
       <c r="H58" t="n">
-        <v>-589.16</v>
+        <v>-589.23</v>
       </c>
       <c r="I58" t="n">
-        <v>-0.23</v>
+        <v>-0.3</v>
       </c>
       <c r="J58" t="n">
         <v>0.5</v>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3494,10 +3494,10 @@
         <v>-435.87</v>
       </c>
       <c r="H59" t="n">
-        <v>-435.91</v>
+        <v>-435.89</v>
       </c>
       <c r="I59" t="n">
-        <v>-0.04</v>
+        <v>-0.02</v>
       </c>
       <c r="J59" t="n">
         <v>0.5</v>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3546,10 +3546,10 @@
         <v>-39.78</v>
       </c>
       <c r="H60" t="n">
-        <v>-40.11</v>
+        <v>-40.1</v>
       </c>
       <c r="I60" t="n">
-        <v>-0.33</v>
+        <v>-0.32</v>
       </c>
       <c r="J60" t="n">
         <v>0.5</v>
@@ -3559,7 +3559,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3571,7 +3571,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>22:17:40</t>
+          <t>22:44:23</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3598,10 +3598,10 @@
         <v>6.5</v>
       </c>
       <c r="H61" t="n">
-        <v>6.74</v>
+        <v>6.75</v>
       </c>
       <c r="I61" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="J61" t="n">
         <v>0.08</v>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>C2609.TXT</t>
+          <t>C2612.TXT</t>
         </is>
       </c>
     </row>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -3727,7 +3727,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3767,7 +3767,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3975,7 +3975,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -3987,7 +3987,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -4027,7 +4027,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -4066,10 +4066,10 @@
         <v>-588.9299999999999</v>
       </c>
       <c r="H70" t="n">
-        <v>-589.24</v>
+        <v>-589.26</v>
       </c>
       <c r="I70" t="n">
-        <v>-0.31</v>
+        <v>-0.33</v>
       </c>
       <c r="J70" t="n">
         <v>0.5</v>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -4131,7 +4131,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -4143,7 +4143,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>22:25:35</t>
+          <t>22:49:55</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -4222,10 +4222,10 @@
         <v>6.5</v>
       </c>
       <c r="H73" t="n">
-        <v>6.77</v>
+        <v>6.74</v>
       </c>
       <c r="I73" t="n">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="J73" t="n">
         <v>0.08</v>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>C2610.TXT</t>
+          <t>C2613.TXT</t>
         </is>
       </c>
     </row>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -4287,7 +4287,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4299,7 +4299,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -4391,7 +4391,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4403,7 +4403,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -4443,7 +4443,7 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4455,7 +4455,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -4495,7 +4495,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -4547,7 +4547,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -4599,7 +4599,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4611,7 +4611,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -4651,7 +4651,7 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4663,7 +4663,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -4690,10 +4690,10 @@
         <v>-588.9299999999999</v>
       </c>
       <c r="H82" t="n">
-        <v>-588.91</v>
+        <v>-589.23</v>
       </c>
       <c r="I82" t="n">
-        <v>0.02</v>
+        <v>-0.3</v>
       </c>
       <c r="J82" t="n">
         <v>0.5</v>
@@ -4703,7 +4703,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4715,7 +4715,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -4742,10 +4742,10 @@
         <v>-435.87</v>
       </c>
       <c r="H83" t="n">
-        <v>-435.88</v>
+        <v>-435.89</v>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
       <c r="J83" t="n">
         <v>0.5</v>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4767,7 +4767,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4794,10 +4794,10 @@
         <v>-39.78</v>
       </c>
       <c r="H84" t="n">
-        <v>-40.05</v>
+        <v>-40.1</v>
       </c>
       <c r="I84" t="n">
-        <v>-0.27</v>
+        <v>-0.32</v>
       </c>
       <c r="J84" t="n">
         <v>0.5</v>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>C2611.TXT</t>
+          <t>C2614.TXT</t>
         </is>
       </c>
     </row>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>22:36:51</t>
+          <t>22:56:01</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -4858,1878 +4858,6 @@
         <v>-0.3</v>
       </c>
       <c r="L85" t="inlineStr">
-        <is>
-          <t>C2611.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G86" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H86" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="I86" t="n">
-        <v>0</v>
-      </c>
-      <c r="J86" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K86" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G87" t="n">
-        <v>-536.17</v>
-      </c>
-      <c r="H87" t="n">
-        <v>-536.17</v>
-      </c>
-      <c r="I87" t="n">
-        <v>0</v>
-      </c>
-      <c r="J87" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K87" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G88" t="n">
-        <v>26.09</v>
-      </c>
-      <c r="H88" t="n">
-        <v>26.09</v>
-      </c>
-      <c r="I88" t="n">
-        <v>0</v>
-      </c>
-      <c r="J88" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K88" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>LOC2</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>SLOT</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>DATUM A2/B2</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G89" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H89" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="I89" t="n">
-        <v>0</v>
-      </c>
-      <c r="J89" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K89" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>LOC2</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>SLOT</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>DATUM A2/B2</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G90" t="n">
-        <v>-71.12</v>
-      </c>
-      <c r="H90" t="n">
-        <v>-71.12</v>
-      </c>
-      <c r="I90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J90" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K90" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G91" t="n">
-        <v>-586.02</v>
-      </c>
-      <c r="H91" t="n">
-        <v>-586.02</v>
-      </c>
-      <c r="I91" t="n">
-        <v>0</v>
-      </c>
-      <c r="J91" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K91" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G92" t="n">
-        <v>-322.77</v>
-      </c>
-      <c r="H92" t="n">
-        <v>-322.77</v>
-      </c>
-      <c r="I92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J92" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K92" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G93" t="n">
-        <v>-71</v>
-      </c>
-      <c r="H93" t="n">
-        <v>-71</v>
-      </c>
-      <c r="I93" t="n">
-        <v>0</v>
-      </c>
-      <c r="J93" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K93" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G94" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H94" t="n">
-        <v>-589.23</v>
-      </c>
-      <c r="I94" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="J94" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K94" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G95" t="n">
-        <v>-435.87</v>
-      </c>
-      <c r="H95" t="n">
-        <v>-435.89</v>
-      </c>
-      <c r="I95" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="J95" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K95" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G96" t="n">
-        <v>-39.78</v>
-      </c>
-      <c r="H96" t="n">
-        <v>-40.1</v>
-      </c>
-      <c r="I96" t="n">
-        <v>-0.32</v>
-      </c>
-      <c r="J96" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K96" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>22:44:23</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G97" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="H97" t="n">
-        <v>6.75</v>
-      </c>
-      <c r="I97" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="J97" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="K97" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>C2612.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G98" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H98" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="I98" t="n">
-        <v>0</v>
-      </c>
-      <c r="J98" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K98" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G99" t="n">
-        <v>-536.17</v>
-      </c>
-      <c r="H99" t="n">
-        <v>-536.17</v>
-      </c>
-      <c r="I99" t="n">
-        <v>0</v>
-      </c>
-      <c r="J99" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K99" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G100" t="n">
-        <v>26.09</v>
-      </c>
-      <c r="H100" t="n">
-        <v>26.09</v>
-      </c>
-      <c r="I100" t="n">
-        <v>0</v>
-      </c>
-      <c r="J100" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K100" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>LOC2</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>SLOT</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>DATUM A2/B2</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G101" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H101" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="I101" t="n">
-        <v>0</v>
-      </c>
-      <c r="J101" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K101" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>LOC2</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>SLOT</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>DATUM A2/B2</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G102" t="n">
-        <v>-71.12</v>
-      </c>
-      <c r="H102" t="n">
-        <v>-71.12</v>
-      </c>
-      <c r="I102" t="n">
-        <v>0</v>
-      </c>
-      <c r="J102" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K102" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G103" t="n">
-        <v>-586.02</v>
-      </c>
-      <c r="H103" t="n">
-        <v>-586.02</v>
-      </c>
-      <c r="I103" t="n">
-        <v>0</v>
-      </c>
-      <c r="J103" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K103" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G104" t="n">
-        <v>-322.77</v>
-      </c>
-      <c r="H104" t="n">
-        <v>-322.77</v>
-      </c>
-      <c r="I104" t="n">
-        <v>0</v>
-      </c>
-      <c r="J104" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K104" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G105" t="n">
-        <v>-71</v>
-      </c>
-      <c r="H105" t="n">
-        <v>-71</v>
-      </c>
-      <c r="I105" t="n">
-        <v>0</v>
-      </c>
-      <c r="J105" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K105" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L105" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G106" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H106" t="n">
-        <v>-589.26</v>
-      </c>
-      <c r="I106" t="n">
-        <v>-0.33</v>
-      </c>
-      <c r="J106" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K106" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L106" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G107" t="n">
-        <v>-435.87</v>
-      </c>
-      <c r="H107" t="n">
-        <v>-435.89</v>
-      </c>
-      <c r="I107" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="J107" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K107" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L107" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G108" t="n">
-        <v>-39.78</v>
-      </c>
-      <c r="H108" t="n">
-        <v>-40.1</v>
-      </c>
-      <c r="I108" t="n">
-        <v>-0.32</v>
-      </c>
-      <c r="J108" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K108" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L108" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>22:49:55</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G109" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="H109" t="n">
-        <v>6.74</v>
-      </c>
-      <c r="I109" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="J109" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="K109" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="L109" t="inlineStr">
-        <is>
-          <t>C2613.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G110" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H110" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="I110" t="n">
-        <v>0</v>
-      </c>
-      <c r="J110" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K110" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L110" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G111" t="n">
-        <v>-536.17</v>
-      </c>
-      <c r="H111" t="n">
-        <v>-536.17</v>
-      </c>
-      <c r="I111" t="n">
-        <v>0</v>
-      </c>
-      <c r="J111" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K111" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L111" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>LOC1</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>PONTO</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>DATUM A3</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G112" t="n">
-        <v>26.09</v>
-      </c>
-      <c r="H112" t="n">
-        <v>26.09</v>
-      </c>
-      <c r="I112" t="n">
-        <v>0</v>
-      </c>
-      <c r="J112" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K112" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>LOC2</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>SLOT</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>DATUM A2/B2</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G113" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H113" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="I113" t="n">
-        <v>0</v>
-      </c>
-      <c r="J113" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K113" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>LOC2</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>SLOT</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>DATUM A2/B2</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G114" t="n">
-        <v>-71.12</v>
-      </c>
-      <c r="H114" t="n">
-        <v>-71.12</v>
-      </c>
-      <c r="I114" t="n">
-        <v>0</v>
-      </c>
-      <c r="J114" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K114" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L114" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G115" t="n">
-        <v>-586.02</v>
-      </c>
-      <c r="H115" t="n">
-        <v>-586.02</v>
-      </c>
-      <c r="I115" t="n">
-        <v>0</v>
-      </c>
-      <c r="J115" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K115" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L115" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G116" t="n">
-        <v>-322.77</v>
-      </c>
-      <c r="H116" t="n">
-        <v>-322.77</v>
-      </c>
-      <c r="I116" t="n">
-        <v>0</v>
-      </c>
-      <c r="J116" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K116" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L116" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>LOC3</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>DATUM A1/B1/C1</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G117" t="n">
-        <v>-71</v>
-      </c>
-      <c r="H117" t="n">
-        <v>-71</v>
-      </c>
-      <c r="I117" t="n">
-        <v>0</v>
-      </c>
-      <c r="J117" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K117" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="L117" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G118" t="n">
-        <v>-588.9299999999999</v>
-      </c>
-      <c r="H118" t="n">
-        <v>-589.23</v>
-      </c>
-      <c r="I118" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="J118" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K118" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L118" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="G119" t="n">
-        <v>-435.87</v>
-      </c>
-      <c r="H119" t="n">
-        <v>-435.89</v>
-      </c>
-      <c r="I119" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="J119" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K119" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L119" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="G120" t="n">
-        <v>-39.78</v>
-      </c>
-      <c r="H120" t="n">
-        <v>-40.1</v>
-      </c>
-      <c r="I120" t="n">
-        <v>-0.32</v>
-      </c>
-      <c r="J120" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K120" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="L120" t="inlineStr">
-        <is>
-          <t>C2614.TXT</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>22:56:01</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>LOC4</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>CÍRCULO</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>CÍR1</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G121" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="H121" t="n">
-        <v>6.73</v>
-      </c>
-      <c r="I121" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="J121" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="K121" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="L121" t="inlineStr">
         <is>
           <t>C2614.TXT</t>
         </is>

</xml_diff>